<commit_message>
EtherCAT sample_app.xlsx file is now readable. [MH3-43715]
</commit_message>
<xml_diff>
--- a/apps/ethercat_counter_foe_app/firmware/src/slave_stack/sample_app.xlsx
+++ b/apps/ethercat_counter_foe_app/firmware/src/slave_stack/sample_app.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EtherCAT\hrisikesh\LAN9252-SPI_SAME54_SDK_V0.1a_FoE_BetaSupport\LAN9252-SPI_SAME54_SDK_V0.1a\SPI Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\microchip\h3\new_ethercat\ethercat\apps\ethercat_counter_foe_app\firmware\src\slave_stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A114F-F11F-4432-8624-590CB4849199}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3298A-B458-4463-AD2D-547D1A138D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="10308" yWindow="2208" windowWidth="4080" windowHeight="6072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="11" r:id="rId1"/>
@@ -142,34 +142,6 @@
   </si>
   <si>
     <t>//0x1C13</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Usage Notes: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- The PDO mapping object and SyncManager assignment object doesn't need to be defined. In that case they are created automatically.
-- The following objects are fixed included in the SSC and shall not be defined in the file : 0x1000, 0x1001, 0x1008, 0x1009, 0x100a, 0x1010, 0x1011, 0x1018, 0x10F0, 0x10F1, 0x10F3, 0x1c00, 0x1c32, 0x1c33
-- Entries less or equal one 8Bit shall not overlap byte borders.
-- Entries greater 8Bit shall always start at an exact word border
-</t>
-    </r>
   </si>
   <si>
     <r>
@@ -331,6 +303,34 @@
   </si>
   <si>
     <t>Trigger</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Usage Notes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- The PDO mapping object and SyncManager assignment object doesn't need to be defined. In that case they are created automatically.
+- The following objects are fixed included in the SSC and shall not be defined in the file : 0x1000, 0x1001, 0x1008, 0x1009, 0x100a, 0x1010, 0x1011, 0x1018, 0x10F0, 0x10F1, 0x10F3, 0x1c00, 0x1c32, 0x1c33
+- Entries less or equal one 8Bit shall not overlap byte borders.
+- Entries greater 8Bit shall always start at an exact word border 
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -800,30 +800,30 @@
   <dimension ref="A1:T902"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+      <pane ySplit="10" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="16" customWidth="1"/>
-    <col min="3" max="5" width="14.6640625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="40.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="16" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.6640625" style="16" customWidth="1"/>
-    <col min="17" max="16384" width="10.6640625" style="16"/>
+    <col min="1" max="1" width="3.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="16" customWidth="1"/>
+    <col min="3" max="5" width="14.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="16" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.7109375" style="16" customWidth="1"/>
+    <col min="17" max="16384" width="10.7109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>18</v>
@@ -836,7 +836,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="21" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
@@ -853,13 +853,13 @@
       <c r="S1" s="17"/>
       <c r="T1" s="17"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
@@ -879,7 +879,7 @@
       <c r="S2" s="17"/>
       <c r="T2" s="17"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
@@ -901,7 +901,7 @@
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="5"/>
@@ -923,7 +923,7 @@
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -945,7 +945,7 @@
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -967,7 +967,7 @@
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -989,7 +989,7 @@
       <c r="S7" s="17"/>
       <c r="T7" s="17"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
         <v>21</v>
@@ -1009,7 +1009,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1027,7 +1027,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="8" t="s">
         <v>0</v>
@@ -1066,16 +1066,16 @@
         <v>5</v>
       </c>
       <c r="N10" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="15" t="s">
         <v>22</v>
@@ -1097,7 +1097,7 @@
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1115,7 +1115,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1133,7 +1133,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
         <v>35</v>
@@ -1155,7 +1155,7 @@
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1173,7 +1173,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="13"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1191,7 +1191,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="13"/>
     </row>
-    <row r="17" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="14" t="s">
         <v>24</v>
@@ -1213,7 +1213,7 @@
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
     </row>
-    <row r="18" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1231,7 +1231,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="13"/>
     </row>
-    <row r="19" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1249,13 +1249,13 @@
       <c r="O19" s="4"/>
       <c r="P19" s="13"/>
     </row>
-    <row r="20" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -1271,7 +1271,7 @@
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
     </row>
-    <row r="21" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1289,7 +1289,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1307,7 +1307,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="13"/>
     </row>
-    <row r="23" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="14" t="s">
         <v>27</v>
@@ -1329,7 +1329,7 @@
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
     </row>
-    <row r="24" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1347,7 +1347,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1365,13 +1365,13 @@
       <c r="O25" s="4"/>
       <c r="P25" s="13"/>
     </row>
-    <row r="26" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -1387,7 +1387,7 @@
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
     </row>
-    <row r="27" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1405,7 +1405,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1423,13 +1423,13 @@
       <c r="O28" s="4"/>
       <c r="P28" s="13"/>
     </row>
-    <row r="29" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -1445,7 +1445,7 @@
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
     </row>
-    <row r="30" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1463,7 +1463,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="13"/>
     </row>
-    <row r="31" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1481,13 +1481,13 @@
       <c r="O31" s="4"/>
       <c r="P31" s="13"/>
     </row>
-    <row r="32" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" s="18" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
@@ -1503,7 +1503,7 @@
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
     </row>
-    <row r="33" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1521,7 +1521,7 @@
       <c r="O33" s="4"/>
       <c r="P33" s="13"/>
     </row>
-    <row r="34" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1539,7 +1539,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="13"/>
     </row>
-    <row r="35" spans="1:16" s="18" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="18" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="14" t="s">
         <v>23</v>
@@ -1561,17 +1561,17 @@
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="D36" s="11"/>
       <c r="F36" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -1579,16 +1579,16 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1596,35 +1596,35 @@
         <v>1</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1642,7 +1642,7 @@
       <c r="O38" s="4"/>
       <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="14" t="s">
         <v>13</v>
@@ -1664,18 +1664,18 @@
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
@@ -1683,16 +1683,16 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1700,35 +1700,35 @@
         <v>1</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1746,7 +1746,7 @@
       <c r="O42" s="4"/>
       <c r="P42" s="13"/>
     </row>
-    <row r="43" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="14" t="s">
         <v>12</v>
@@ -1768,7 +1768,7 @@
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1786,7 +1786,7 @@
       <c r="O44" s="4"/>
       <c r="P44" s="13"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1804,7 +1804,7 @@
       <c r="O45" s="4"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="46" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="14" t="s">
         <v>14</v>
@@ -1826,7 +1826,7 @@
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1844,7 +1844,7 @@
       <c r="O47" s="4"/>
       <c r="P47" s="13"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1862,7 +1862,7 @@
       <c r="O48" s="4"/>
       <c r="P48" s="13"/>
     </row>
-    <row r="49" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
         <v>15</v>
@@ -1884,7 +1884,7 @@
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1902,7 +1902,7 @@
       <c r="O50" s="4"/>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1920,7 +1920,7 @@
       <c r="O51" s="4"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1938,7 +1938,7 @@
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1956,7 +1956,7 @@
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1974,7 +1974,7 @@
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1992,7 +1992,7 @@
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2010,7 +2010,7 @@
       <c r="O56" s="4"/>
       <c r="P56" s="4"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2028,7 +2028,7 @@
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2046,7 +2046,7 @@
       <c r="O58" s="4"/>
       <c r="P58" s="4"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2064,7 +2064,7 @@
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2082,7 +2082,7 @@
       <c r="O60" s="4"/>
       <c r="P60" s="4"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2100,7 +2100,7 @@
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2118,2524 +2118,2524 @@
       <c r="O62" s="4"/>
       <c r="P62" s="4"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C200" s="4"/>
     </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C201" s="4"/>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C202" s="4"/>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C203" s="4"/>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C204" s="4"/>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C205" s="4"/>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C206" s="4"/>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C207" s="4"/>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C208" s="4"/>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C209" s="4"/>
     </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C210" s="4"/>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C211" s="4"/>
     </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C212" s="4"/>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C214" s="4"/>
     </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C215" s="4"/>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C216" s="4"/>
     </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C217" s="4"/>
     </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C218" s="4"/>
     </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C219" s="4"/>
     </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C220" s="4"/>
     </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C221" s="4"/>
     </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C222" s="4"/>
     </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C223" s="4"/>
     </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C224" s="4"/>
     </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C225" s="4"/>
     </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C226" s="4"/>
     </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C227" s="4"/>
     </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C228" s="4"/>
     </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C229" s="4"/>
     </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C230" s="4"/>
     </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C231" s="4"/>
     </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C232" s="4"/>
     </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C233" s="4"/>
     </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C234" s="4"/>
     </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C235" s="4"/>
     </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C236" s="4"/>
     </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C238" s="4"/>
     </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C239" s="4"/>
     </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C240" s="4"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C241" s="4"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C242" s="4"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C243" s="4"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C244" s="4"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C245" s="4"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C246" s="4"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C247" s="4"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C248" s="4"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C249" s="4"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C250" s="4"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C251" s="4"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C252" s="4"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C253" s="4"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C254" s="4"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C255" s="4"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C256" s="4"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C257" s="4"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C258" s="4"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C259" s="4"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C260" s="4"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C261" s="4"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C262" s="4"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C263" s="4"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C264" s="4"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C265" s="4"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C266" s="4"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C267" s="4"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C268" s="4"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C269" s="4"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C270" s="4"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C271" s="4"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C272" s="4"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C275" s="4"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C276" s="4"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C277" s="4"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C278" s="4"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C279" s="4"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C280" s="4"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C281" s="4"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C282" s="4"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C283" s="4"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C284" s="4"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C285" s="4"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C286" s="4"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C287" s="4"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C288" s="4"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C289" s="4"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C290" s="4"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C291" s="4"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C292" s="4"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C293" s="4"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C294" s="4"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C295" s="4"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C296" s="4"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C297" s="4"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C298" s="4"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C299" s="4"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C300" s="4"/>
     </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C301" s="4"/>
     </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C302" s="4"/>
     </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C303" s="4"/>
     </row>
-    <row r="304" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C304" s="4"/>
     </row>
-    <row r="305" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C305" s="4"/>
     </row>
-    <row r="306" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C306" s="4"/>
     </row>
-    <row r="307" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C307" s="4"/>
     </row>
-    <row r="308" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C308" s="4"/>
     </row>
-    <row r="309" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C309" s="4"/>
     </row>
-    <row r="310" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C310" s="4"/>
     </row>
-    <row r="311" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C311" s="4"/>
     </row>
-    <row r="312" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C312" s="4"/>
     </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C313" s="4"/>
     </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C314" s="4"/>
     </row>
-    <row r="315" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C315" s="4"/>
     </row>
-    <row r="316" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C316" s="4"/>
     </row>
-    <row r="317" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C317" s="4"/>
     </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C318" s="4"/>
     </row>
-    <row r="319" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C319" s="4"/>
     </row>
-    <row r="320" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C320" s="4"/>
     </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321" s="4"/>
     </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322" s="4"/>
     </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323" s="4"/>
     </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C324" s="4"/>
     </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325" s="4"/>
     </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C326" s="4"/>
     </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C327" s="4"/>
     </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C328" s="4"/>
     </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329" s="4"/>
     </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C330" s="4"/>
     </row>
-    <row r="331" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C331" s="4"/>
     </row>
-    <row r="332" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C332" s="4"/>
     </row>
-    <row r="333" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C333" s="4"/>
     </row>
-    <row r="334" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C334" s="4"/>
     </row>
-    <row r="335" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C335" s="4"/>
     </row>
-    <row r="336" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C336" s="4"/>
     </row>
-    <row r="337" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="337" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C337" s="4"/>
     </row>
-    <row r="338" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="338" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C338" s="4"/>
     </row>
-    <row r="339" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="339" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C339" s="4"/>
     </row>
-    <row r="340" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="340" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C340" s="4"/>
     </row>
-    <row r="341" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="341" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C341" s="4"/>
     </row>
-    <row r="342" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="342" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C342" s="4"/>
     </row>
-    <row r="343" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="343" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C343" s="4"/>
     </row>
-    <row r="344" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="344" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C344" s="4"/>
     </row>
-    <row r="345" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="345" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C345" s="4"/>
     </row>
-    <row r="346" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="346" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C346" s="4"/>
     </row>
-    <row r="347" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="347" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C347" s="4"/>
     </row>
-    <row r="348" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="348" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C348" s="4"/>
     </row>
-    <row r="349" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="349" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C349" s="4"/>
     </row>
-    <row r="350" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="350" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C350" s="4"/>
     </row>
-    <row r="351" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="351" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C351" s="4"/>
     </row>
-    <row r="352" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="352" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C352" s="4"/>
     </row>
-    <row r="353" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="353" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C353" s="4"/>
     </row>
-    <row r="354" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="354" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="355" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="356" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="357" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="358" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="359" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="360" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="361" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="362" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="363" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="364" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="365" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C365" s="4"/>
     </row>
-    <row r="366" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="366" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="367" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C367" s="4"/>
     </row>
-    <row r="368" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="368" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="369" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C369" s="4"/>
     </row>
-    <row r="370" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="370" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C371" s="4"/>
     </row>
-    <row r="372" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C373" s="4"/>
     </row>
-    <row r="374" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="374" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C375" s="4"/>
     </row>
-    <row r="376" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="376" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C377" s="4"/>
     </row>
-    <row r="378" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="378" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C379" s="4"/>
     </row>
-    <row r="380" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="381" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C381" s="4"/>
     </row>
-    <row r="382" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="382" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C383" s="4"/>
     </row>
-    <row r="384" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="385" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C385" s="4"/>
     </row>
-    <row r="386" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="386" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="387" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C387" s="4"/>
     </row>
-    <row r="388" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="388" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C388" s="4"/>
     </row>
-    <row r="389" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="389" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C389" s="4"/>
     </row>
-    <row r="390" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="390" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C390" s="4"/>
     </row>
-    <row r="391" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="391" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C391" s="4"/>
     </row>
-    <row r="392" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="392" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C392" s="4"/>
     </row>
-    <row r="393" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="393" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C393" s="4"/>
     </row>
-    <row r="394" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="394" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C394" s="4"/>
     </row>
-    <row r="395" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="395" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C395" s="4"/>
     </row>
-    <row r="396" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="396" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C396" s="4"/>
     </row>
-    <row r="397" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="397" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C397" s="4"/>
     </row>
-    <row r="398" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="398" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C398" s="4"/>
     </row>
-    <row r="399" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="399" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C399" s="4"/>
     </row>
-    <row r="400" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="400" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="401" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="402" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C402" s="4"/>
     </row>
-    <row r="403" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="403" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C403" s="4"/>
     </row>
-    <row r="404" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="404" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C404" s="4"/>
     </row>
-    <row r="405" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="405" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C405" s="4"/>
     </row>
-    <row r="406" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="406" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C406" s="4"/>
     </row>
-    <row r="407" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="407" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C407" s="4"/>
     </row>
-    <row r="408" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="408" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="409" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="410" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C410" s="4"/>
     </row>
-    <row r="411" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="411" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C411" s="4"/>
     </row>
-    <row r="412" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="412" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C412" s="4"/>
     </row>
-    <row r="413" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="413" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C413" s="4"/>
     </row>
-    <row r="414" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="414" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C414" s="4"/>
     </row>
-    <row r="415" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="415" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C415" s="4"/>
     </row>
-    <row r="416" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="416" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C416" s="4"/>
     </row>
-    <row r="417" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="417" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C417" s="4"/>
     </row>
-    <row r="418" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="418" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C418" s="4"/>
     </row>
-    <row r="419" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="419" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C419" s="4"/>
     </row>
-    <row r="420" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="420" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C420" s="4"/>
     </row>
-    <row r="421" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="421" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C421" s="4"/>
     </row>
-    <row r="422" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="422" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C422" s="4"/>
     </row>
-    <row r="423" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="423" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C423" s="4"/>
     </row>
-    <row r="424" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="424" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C424" s="4"/>
     </row>
-    <row r="425" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="425" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C425" s="4"/>
     </row>
-    <row r="426" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="426" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C426" s="4"/>
     </row>
-    <row r="427" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="427" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C427" s="4"/>
     </row>
-    <row r="428" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="428" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C428" s="4"/>
     </row>
-    <row r="429" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="429" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C429" s="4"/>
     </row>
-    <row r="430" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="430" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C430" s="4"/>
     </row>
-    <row r="431" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="431" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C431" s="4"/>
     </row>
-    <row r="432" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="432" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C432" s="4"/>
     </row>
-    <row r="433" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="433" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C433" s="4"/>
     </row>
-    <row r="434" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="434" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C434" s="4"/>
     </row>
-    <row r="435" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="435" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C435" s="4"/>
     </row>
-    <row r="436" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="436" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C436" s="4"/>
     </row>
-    <row r="437" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="437" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C437" s="4"/>
     </row>
-    <row r="438" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="438" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C438" s="4"/>
     </row>
-    <row r="439" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="439" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C439" s="4"/>
     </row>
-    <row r="440" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="440" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C440" s="4"/>
     </row>
-    <row r="441" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="441" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C441" s="4"/>
     </row>
-    <row r="442" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="442" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C442" s="4"/>
     </row>
-    <row r="443" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="443" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C443" s="4"/>
     </row>
-    <row r="444" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="444" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C444" s="4"/>
     </row>
-    <row r="445" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="445" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C445" s="4"/>
     </row>
-    <row r="446" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="446" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C446" s="4"/>
     </row>
-    <row r="447" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="447" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C447" s="4"/>
     </row>
-    <row r="448" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="448" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C448" s="4"/>
     </row>
-    <row r="449" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="449" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C449" s="4"/>
     </row>
-    <row r="450" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="450" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C450" s="4"/>
     </row>
-    <row r="451" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="451" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C451" s="4"/>
     </row>
-    <row r="452" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="452" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C452" s="4"/>
     </row>
-    <row r="453" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="453" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C453" s="4"/>
     </row>
-    <row r="454" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="454" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C454" s="4"/>
     </row>
-    <row r="455" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="455" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C455" s="4"/>
     </row>
-    <row r="456" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="456" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C456" s="4"/>
     </row>
-    <row r="457" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="457" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C457" s="4"/>
     </row>
-    <row r="458" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="458" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C458" s="4"/>
     </row>
-    <row r="459" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="459" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C459" s="4"/>
     </row>
-    <row r="460" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="460" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C460" s="4"/>
     </row>
-    <row r="461" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="461" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C461" s="4"/>
     </row>
-    <row r="462" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="462" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C462" s="4"/>
     </row>
-    <row r="463" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="463" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C463" s="4"/>
     </row>
-    <row r="464" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="464" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C464" s="4"/>
     </row>
-    <row r="465" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="465" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C465" s="4"/>
     </row>
-    <row r="466" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="466" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C466" s="4"/>
     </row>
-    <row r="467" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="467" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C467" s="4"/>
     </row>
-    <row r="468" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="468" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C468" s="4"/>
     </row>
-    <row r="469" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="469" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C469" s="4"/>
     </row>
-    <row r="470" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="470" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C470" s="4"/>
     </row>
-    <row r="471" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="471" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="472" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C472" s="4"/>
     </row>
-    <row r="473" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="473" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C473" s="4"/>
     </row>
-    <row r="474" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="474" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C474" s="4"/>
     </row>
-    <row r="475" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="475" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C475" s="4"/>
     </row>
-    <row r="476" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="476" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C476" s="4"/>
     </row>
-    <row r="477" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="477" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C477" s="4"/>
     </row>
-    <row r="478" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="478" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C478" s="4"/>
     </row>
-    <row r="479" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="479" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C479" s="4"/>
     </row>
-    <row r="480" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="480" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C480" s="4"/>
     </row>
-    <row r="481" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="481" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C481" s="4"/>
     </row>
-    <row r="482" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="482" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C482" s="4"/>
     </row>
-    <row r="483" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="483" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C483" s="4"/>
     </row>
-    <row r="484" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="484" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C484" s="4"/>
     </row>
-    <row r="485" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="485" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C485" s="4"/>
     </row>
-    <row r="486" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="486" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C486" s="4"/>
     </row>
-    <row r="487" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="487" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C487" s="4"/>
     </row>
-    <row r="488" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="488" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C488" s="4"/>
     </row>
-    <row r="489" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="489" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C489" s="4"/>
     </row>
-    <row r="490" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="490" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C490" s="4"/>
     </row>
-    <row r="491" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="491" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C491" s="4"/>
     </row>
-    <row r="492" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="492" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C492" s="4"/>
     </row>
-    <row r="493" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="493" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C493" s="4"/>
     </row>
-    <row r="494" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="494" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C494" s="4"/>
     </row>
-    <row r="495" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="495" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C495" s="4"/>
     </row>
-    <row r="496" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="496" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C496" s="4"/>
     </row>
-    <row r="497" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="497" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C497" s="4"/>
     </row>
-    <row r="498" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="498" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C498" s="4"/>
     </row>
-    <row r="499" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="499" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C499" s="4"/>
     </row>
-    <row r="500" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="500" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C500" s="4"/>
     </row>
-    <row r="501" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="501" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C501" s="4"/>
     </row>
-    <row r="502" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="502" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C502" s="4"/>
     </row>
-    <row r="503" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="503" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C503" s="4"/>
     </row>
-    <row r="504" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="504" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C504" s="4"/>
     </row>
-    <row r="505" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="505" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C505" s="4"/>
     </row>
-    <row r="506" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="506" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C506" s="4"/>
     </row>
-    <row r="507" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="507" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C507" s="4"/>
     </row>
-    <row r="508" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="508" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C508" s="4"/>
     </row>
-    <row r="509" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="509" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C509" s="4"/>
     </row>
-    <row r="510" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="510" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C510" s="4"/>
     </row>
-    <row r="511" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="511" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C511" s="4"/>
     </row>
-    <row r="512" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="512" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C512" s="4"/>
     </row>
-    <row r="513" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="513" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C513" s="4"/>
     </row>
-    <row r="514" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="514" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C514" s="4"/>
     </row>
-    <row r="515" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="515" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C515" s="4"/>
     </row>
-    <row r="516" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="516" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C516" s="4"/>
     </row>
-    <row r="517" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="517" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C517" s="4"/>
     </row>
-    <row r="518" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="518" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C518" s="4"/>
     </row>
-    <row r="519" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="519" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C519" s="4"/>
     </row>
-    <row r="520" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="520" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C520" s="4"/>
     </row>
-    <row r="521" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="521" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C521" s="4"/>
     </row>
-    <row r="522" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="522" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C522" s="4"/>
     </row>
-    <row r="523" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="523" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C523" s="4"/>
     </row>
-    <row r="524" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="524" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C524" s="4"/>
     </row>
-    <row r="525" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="525" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C525" s="4"/>
     </row>
-    <row r="526" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="526" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C526" s="4"/>
     </row>
-    <row r="527" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="527" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C527" s="4"/>
     </row>
-    <row r="528" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="528" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C528" s="4"/>
     </row>
-    <row r="529" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="529" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C529" s="4"/>
     </row>
-    <row r="530" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="530" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C530" s="4"/>
     </row>
-    <row r="531" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="531" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C531" s="4"/>
     </row>
-    <row r="532" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="532" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C532" s="4"/>
     </row>
-    <row r="533" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="533" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C533" s="4"/>
     </row>
-    <row r="534" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="534" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C534" s="4"/>
     </row>
-    <row r="535" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="535" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C535" s="4"/>
     </row>
-    <row r="536" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="536" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C536" s="4"/>
     </row>
-    <row r="537" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="537" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C537" s="4"/>
     </row>
-    <row r="538" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="538" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C538" s="4"/>
     </row>
-    <row r="539" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="539" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C539" s="4"/>
     </row>
-    <row r="540" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="540" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C540" s="4"/>
     </row>
-    <row r="541" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="541" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C541" s="4"/>
     </row>
-    <row r="542" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="542" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C542" s="4"/>
     </row>
-    <row r="543" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="543" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C543" s="4"/>
     </row>
-    <row r="544" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="544" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C544" s="4"/>
     </row>
-    <row r="545" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="545" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C545" s="4"/>
     </row>
-    <row r="546" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="546" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C546" s="4"/>
     </row>
-    <row r="547" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="547" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C547" s="4"/>
     </row>
-    <row r="548" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="548" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C548" s="4"/>
     </row>
-    <row r="549" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="549" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C549" s="4"/>
     </row>
-    <row r="550" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="550" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C550" s="4"/>
     </row>
-    <row r="551" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="551" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C551" s="4"/>
     </row>
-    <row r="552" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="552" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C552" s="4"/>
     </row>
-    <row r="553" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="553" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C553" s="4"/>
     </row>
-    <row r="554" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="554" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C554" s="4"/>
     </row>
-    <row r="555" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="555" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C555" s="4"/>
     </row>
-    <row r="556" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="556" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C556" s="4"/>
     </row>
-    <row r="557" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="557" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C557" s="4"/>
     </row>
-    <row r="558" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="558" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C558" s="4"/>
     </row>
-    <row r="559" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="559" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C559" s="4"/>
     </row>
-    <row r="560" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="560" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C560" s="4"/>
     </row>
-    <row r="561" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="561" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C561" s="4"/>
     </row>
-    <row r="562" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="562" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C562" s="4"/>
     </row>
-    <row r="563" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="563" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C563" s="4"/>
     </row>
-    <row r="564" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="564" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C564" s="4"/>
     </row>
-    <row r="565" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="565" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C565" s="4"/>
     </row>
-    <row r="566" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="566" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C566" s="4"/>
     </row>
-    <row r="567" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="567" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C567" s="4"/>
     </row>
-    <row r="568" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="568" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C568" s="4"/>
     </row>
-    <row r="569" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="569" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C569" s="4"/>
     </row>
-    <row r="570" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="570" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C570" s="4"/>
     </row>
-    <row r="571" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="571" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C571" s="4"/>
     </row>
-    <row r="572" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="572" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C572" s="4"/>
     </row>
-    <row r="573" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="573" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C573" s="4"/>
     </row>
-    <row r="574" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="574" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C574" s="4"/>
     </row>
-    <row r="575" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="575" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C575" s="4"/>
     </row>
-    <row r="576" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C576" s="4"/>
     </row>
-    <row r="577" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="577" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C577" s="4"/>
     </row>
-    <row r="578" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="578" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C578" s="4"/>
     </row>
-    <row r="579" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="579" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C579" s="4"/>
     </row>
-    <row r="580" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="580" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C580" s="4"/>
     </row>
-    <row r="581" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="581" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C581" s="4"/>
     </row>
-    <row r="582" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="582" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C582" s="4"/>
     </row>
-    <row r="583" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="583" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C583" s="4"/>
     </row>
-    <row r="584" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="584" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C584" s="4"/>
     </row>
-    <row r="585" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="585" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C585" s="4"/>
     </row>
-    <row r="586" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="586" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C586" s="4"/>
     </row>
-    <row r="587" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="587" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C587" s="4"/>
     </row>
-    <row r="588" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="588" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C588" s="4"/>
     </row>
-    <row r="589" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="589" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C589" s="4"/>
     </row>
-    <row r="590" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="590" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C590" s="4"/>
     </row>
-    <row r="591" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="591" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C591" s="4"/>
     </row>
-    <row r="592" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="592" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C592" s="4"/>
     </row>
-    <row r="593" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="593" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C593" s="4"/>
     </row>
-    <row r="594" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="594" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C594" s="4"/>
     </row>
-    <row r="595" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="595" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C595" s="4"/>
     </row>
-    <row r="596" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="596" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C596" s="4"/>
     </row>
-    <row r="597" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="597" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C597" s="4"/>
     </row>
-    <row r="598" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="598" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C598" s="4"/>
     </row>
-    <row r="599" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="599" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C599" s="4"/>
     </row>
-    <row r="600" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="600" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C600" s="4"/>
     </row>
-    <row r="601" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="601" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C601" s="4"/>
     </row>
-    <row r="602" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="602" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C602" s="4"/>
     </row>
-    <row r="603" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="603" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C603" s="4"/>
     </row>
-    <row r="604" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="604" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C604" s="4"/>
     </row>
-    <row r="605" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="605" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C605" s="4"/>
     </row>
-    <row r="606" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="606" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C606" s="4"/>
     </row>
-    <row r="607" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="607" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C607" s="4"/>
     </row>
-    <row r="608" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="608" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C608" s="4"/>
     </row>
-    <row r="609" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="609" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C609" s="4"/>
     </row>
-    <row r="610" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="610" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C610" s="4"/>
     </row>
-    <row r="611" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="611" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C611" s="4"/>
     </row>
-    <row r="612" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="612" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C612" s="4"/>
     </row>
-    <row r="613" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="613" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C613" s="4"/>
     </row>
-    <row r="614" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="614" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C614" s="4"/>
     </row>
-    <row r="615" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="615" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C615" s="4"/>
     </row>
-    <row r="616" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="616" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C616" s="4"/>
     </row>
-    <row r="617" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="617" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C617" s="4"/>
     </row>
-    <row r="618" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="618" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C618" s="4"/>
     </row>
-    <row r="619" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="619" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C619" s="4"/>
     </row>
-    <row r="620" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="620" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C620" s="4"/>
     </row>
-    <row r="621" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="621" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C621" s="4"/>
     </row>
-    <row r="622" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="622" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C622" s="4"/>
     </row>
-    <row r="623" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="623" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C623" s="4"/>
     </row>
-    <row r="624" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="624" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C624" s="4"/>
     </row>
-    <row r="625" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="625" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C625" s="4"/>
     </row>
-    <row r="626" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="626" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C626" s="4"/>
     </row>
-    <row r="627" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="627" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C627" s="4"/>
     </row>
-    <row r="628" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="628" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C628" s="4"/>
     </row>
-    <row r="629" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="629" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C629" s="4"/>
     </row>
-    <row r="630" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="630" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C630" s="4"/>
     </row>
-    <row r="631" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="631" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C631" s="4"/>
     </row>
-    <row r="632" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="632" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C632" s="4"/>
     </row>
-    <row r="633" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="633" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C633" s="4"/>
     </row>
-    <row r="634" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="634" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C634" s="4"/>
     </row>
-    <row r="635" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="635" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C635" s="4"/>
     </row>
-    <row r="636" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="636" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C636" s="4"/>
     </row>
-    <row r="637" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="637" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C637" s="4"/>
     </row>
-    <row r="638" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="638" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C638" s="4"/>
     </row>
-    <row r="639" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="639" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C639" s="4"/>
     </row>
-    <row r="640" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="640" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C640" s="4"/>
     </row>
-    <row r="641" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="641" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C641" s="4"/>
     </row>
-    <row r="642" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="642" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C642" s="4"/>
     </row>
-    <row r="643" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="643" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C643" s="4"/>
     </row>
-    <row r="644" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="644" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C644" s="4"/>
     </row>
-    <row r="645" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="645" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C645" s="4"/>
     </row>
-    <row r="646" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="646" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C646" s="4"/>
     </row>
-    <row r="647" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="647" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C647" s="4"/>
     </row>
-    <row r="648" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="648" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C648" s="4"/>
     </row>
-    <row r="649" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="649" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C649" s="4"/>
     </row>
-    <row r="650" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="650" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C650" s="4"/>
     </row>
-    <row r="651" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="651" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C651" s="4"/>
     </row>
-    <row r="652" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="652" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C652" s="4"/>
     </row>
-    <row r="653" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="653" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C653" s="4"/>
     </row>
-    <row r="654" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="654" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C654" s="4"/>
     </row>
-    <row r="655" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="655" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C655" s="4"/>
     </row>
-    <row r="656" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="656" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C656" s="4"/>
     </row>
-    <row r="657" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="657" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C657" s="4"/>
     </row>
-    <row r="658" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="658" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C658" s="4"/>
     </row>
-    <row r="659" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="659" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C659" s="4"/>
     </row>
-    <row r="660" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="660" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C660" s="4"/>
     </row>
-    <row r="661" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="661" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C661" s="4"/>
     </row>
-    <row r="662" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="662" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C662" s="4"/>
     </row>
-    <row r="663" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="663" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C663" s="4"/>
     </row>
-    <row r="664" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="664" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C664" s="4"/>
     </row>
-    <row r="665" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="665" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C665" s="4"/>
     </row>
-    <row r="666" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="666" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C666" s="4"/>
     </row>
-    <row r="667" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="667" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C667" s="4"/>
     </row>
-    <row r="668" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="668" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C668" s="4"/>
     </row>
-    <row r="669" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="669" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C669" s="4"/>
     </row>
-    <row r="670" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="670" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C670" s="4"/>
     </row>
-    <row r="671" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="671" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C671" s="4"/>
     </row>
-    <row r="672" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="672" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C672" s="4"/>
     </row>
-    <row r="673" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="673" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C673" s="4"/>
     </row>
-    <row r="674" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="674" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C674" s="4"/>
     </row>
-    <row r="675" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="675" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C675" s="4"/>
     </row>
-    <row r="676" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="676" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C676" s="4"/>
     </row>
-    <row r="677" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="677" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C677" s="4"/>
     </row>
-    <row r="678" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="678" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C678" s="4"/>
     </row>
-    <row r="679" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="679" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C679" s="4"/>
     </row>
-    <row r="680" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="680" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C680" s="4"/>
     </row>
-    <row r="681" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="681" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C681" s="4"/>
     </row>
-    <row r="682" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="682" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C682" s="4"/>
     </row>
-    <row r="683" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="683" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C683" s="4"/>
     </row>
-    <row r="684" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="684" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C684" s="4"/>
     </row>
-    <row r="685" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="685" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C685" s="4"/>
     </row>
-    <row r="686" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="686" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C686" s="4"/>
     </row>
-    <row r="687" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="687" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C687" s="4"/>
     </row>
-    <row r="688" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="688" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C688" s="4"/>
     </row>
-    <row r="689" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="689" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C689" s="4"/>
     </row>
-    <row r="690" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="690" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C690" s="4"/>
     </row>
-    <row r="691" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="691" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C691" s="4"/>
     </row>
-    <row r="692" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="692" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C692" s="4"/>
     </row>
-    <row r="693" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="693" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C693" s="4"/>
     </row>
-    <row r="694" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="694" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C694" s="4"/>
     </row>
-    <row r="695" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="695" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C695" s="4"/>
     </row>
-    <row r="696" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="696" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C696" s="4"/>
     </row>
-    <row r="697" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="697" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C697" s="4"/>
     </row>
-    <row r="698" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="698" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C698" s="4"/>
     </row>
-    <row r="699" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="699" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C699" s="4"/>
     </row>
-    <row r="700" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="700" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C700" s="4"/>
     </row>
-    <row r="701" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="701" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C701" s="4"/>
     </row>
-    <row r="702" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="702" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C702" s="4"/>
     </row>
-    <row r="703" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="703" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C703" s="4"/>
     </row>
-    <row r="704" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="704" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C704" s="4"/>
     </row>
-    <row r="705" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="705" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C705" s="4"/>
     </row>
-    <row r="706" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="706" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C706" s="4"/>
     </row>
-    <row r="707" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="707" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C707" s="4"/>
     </row>
-    <row r="708" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="708" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C708" s="4"/>
     </row>
-    <row r="709" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="709" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C709" s="4"/>
     </row>
-    <row r="710" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="710" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C710" s="4"/>
     </row>
-    <row r="711" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="711" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C711" s="4"/>
     </row>
-    <row r="712" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="712" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C712" s="4"/>
     </row>
-    <row r="713" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="713" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C713" s="4"/>
     </row>
-    <row r="714" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="714" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C714" s="4"/>
     </row>
-    <row r="715" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="715" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C715" s="4"/>
     </row>
-    <row r="716" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="716" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C716" s="4"/>
     </row>
-    <row r="717" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="717" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C717" s="4"/>
     </row>
-    <row r="718" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="718" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C718" s="4"/>
     </row>
-    <row r="719" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="719" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C719" s="4"/>
     </row>
-    <row r="720" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="720" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C720" s="4"/>
     </row>
-    <row r="721" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="721" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C721" s="4"/>
     </row>
-    <row r="722" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="722" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C722" s="4"/>
     </row>
-    <row r="723" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="723" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C723" s="4"/>
     </row>
-    <row r="724" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="724" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C724" s="4"/>
     </row>
-    <row r="725" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="725" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C725" s="4"/>
     </row>
-    <row r="726" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="726" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C726" s="4"/>
     </row>
-    <row r="727" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="727" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C727" s="4"/>
     </row>
-    <row r="728" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="728" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C728" s="4"/>
     </row>
-    <row r="729" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="729" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C729" s="4"/>
     </row>
-    <row r="730" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="730" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C730" s="4"/>
     </row>
-    <row r="731" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="731" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C731" s="4"/>
     </row>
-    <row r="732" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="732" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C732" s="4"/>
     </row>
-    <row r="733" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="733" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C733" s="4"/>
     </row>
-    <row r="734" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="734" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C734" s="4"/>
     </row>
-    <row r="735" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="735" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C735" s="4"/>
     </row>
-    <row r="736" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="736" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C736" s="4"/>
     </row>
-    <row r="737" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="737" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C737" s="4"/>
     </row>
-    <row r="738" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="738" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C738" s="4"/>
     </row>
-    <row r="739" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="739" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C739" s="4"/>
     </row>
-    <row r="740" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="740" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C740" s="4"/>
     </row>
-    <row r="741" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="741" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C741" s="4"/>
     </row>
-    <row r="742" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="742" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C742" s="4"/>
     </row>
-    <row r="743" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="743" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C743" s="4"/>
     </row>
-    <row r="744" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="744" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C744" s="4"/>
     </row>
-    <row r="745" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="745" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C745" s="4"/>
     </row>
-    <row r="746" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="746" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C746" s="4"/>
     </row>
-    <row r="747" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="747" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C747" s="4"/>
     </row>
-    <row r="748" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="748" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C748" s="4"/>
     </row>
-    <row r="749" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="749" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C749" s="4"/>
     </row>
-    <row r="750" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="750" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C750" s="4"/>
     </row>
-    <row r="751" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="751" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C751" s="4"/>
     </row>
-    <row r="752" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="752" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C752" s="4"/>
     </row>
-    <row r="753" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="753" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C753" s="4"/>
     </row>
-    <row r="754" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="754" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C754" s="4"/>
     </row>
-    <row r="755" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="755" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C755" s="4"/>
     </row>
-    <row r="756" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="756" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C756" s="4"/>
     </row>
-    <row r="757" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="757" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C757" s="4"/>
     </row>
-    <row r="758" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="758" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C758" s="4"/>
     </row>
-    <row r="759" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="759" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C759" s="4"/>
     </row>
-    <row r="760" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="760" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C760" s="4"/>
     </row>
-    <row r="761" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="761" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C761" s="4"/>
     </row>
-    <row r="762" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="762" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C762" s="4"/>
     </row>
-    <row r="763" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="763" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C763" s="4"/>
     </row>
-    <row r="764" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="764" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C764" s="4"/>
     </row>
-    <row r="765" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="765" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C765" s="4"/>
     </row>
-    <row r="766" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="766" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C766" s="4"/>
     </row>
-    <row r="767" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="767" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C767" s="4"/>
     </row>
-    <row r="768" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="768" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C768" s="4"/>
     </row>
-    <row r="769" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="769" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C769" s="4"/>
     </row>
-    <row r="770" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="770" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C770" s="4"/>
     </row>
-    <row r="771" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="771" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C771" s="4"/>
     </row>
-    <row r="772" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="772" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C772" s="4"/>
     </row>
-    <row r="773" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="773" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C773" s="4"/>
     </row>
-    <row r="774" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="774" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C774" s="4"/>
     </row>
-    <row r="775" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="775" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C775" s="4"/>
     </row>
-    <row r="776" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="776" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C776" s="4"/>
     </row>
-    <row r="777" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="777" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C777" s="4"/>
     </row>
-    <row r="778" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="778" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C778" s="4"/>
     </row>
-    <row r="779" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="779" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C779" s="4"/>
     </row>
-    <row r="780" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="780" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C780" s="4"/>
     </row>
-    <row r="781" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="781" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C781" s="4"/>
     </row>
-    <row r="782" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="782" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C782" s="4"/>
     </row>
-    <row r="783" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="783" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C783" s="4"/>
     </row>
-    <row r="784" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="784" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C784" s="4"/>
     </row>
-    <row r="785" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="785" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C785" s="4"/>
     </row>
-    <row r="786" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="786" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C786" s="4"/>
     </row>
-    <row r="787" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="787" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C787" s="4"/>
     </row>
-    <row r="788" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="788" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C788" s="4"/>
     </row>
-    <row r="789" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="789" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C789" s="4"/>
     </row>
-    <row r="790" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="790" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C790" s="4"/>
     </row>
-    <row r="791" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="791" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C791" s="4"/>
     </row>
-    <row r="792" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="792" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C792" s="4"/>
     </row>
-    <row r="793" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="793" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C793" s="4"/>
     </row>
-    <row r="794" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="794" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C794" s="4"/>
     </row>
-    <row r="795" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="795" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C795" s="4"/>
     </row>
-    <row r="796" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="796" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C796" s="4"/>
     </row>
-    <row r="797" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="797" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C797" s="4"/>
     </row>
-    <row r="798" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="798" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C798" s="4"/>
     </row>
-    <row r="799" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="799" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C799" s="4"/>
     </row>
-    <row r="800" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="800" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C800" s="4"/>
     </row>
-    <row r="801" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="801" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C801" s="4"/>
     </row>
-    <row r="802" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="802" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C802" s="4"/>
     </row>
-    <row r="803" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="803" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C803" s="4"/>
     </row>
-    <row r="804" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="804" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C804" s="4"/>
     </row>
-    <row r="805" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="805" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C805" s="4"/>
     </row>
-    <row r="806" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="806" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C806" s="4"/>
     </row>
-    <row r="807" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="807" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C807" s="4"/>
     </row>
-    <row r="808" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="808" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C808" s="4"/>
     </row>
-    <row r="809" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="809" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C809" s="4"/>
     </row>
-    <row r="810" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="810" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C810" s="4"/>
     </row>
-    <row r="811" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="811" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C811" s="4"/>
     </row>
-    <row r="812" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="812" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C812" s="4"/>
     </row>
-    <row r="813" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="813" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C813" s="4"/>
     </row>
-    <row r="814" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="814" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C814" s="4"/>
     </row>
-    <row r="815" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="815" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C815" s="4"/>
     </row>
-    <row r="816" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="816" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C816" s="4"/>
     </row>
-    <row r="817" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="817" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C817" s="4"/>
     </row>
-    <row r="818" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="818" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C818" s="4"/>
     </row>
-    <row r="819" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="819" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C819" s="4"/>
     </row>
-    <row r="820" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="820" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C820" s="4"/>
     </row>
-    <row r="821" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="821" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C821" s="4"/>
     </row>
-    <row r="822" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="822" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C822" s="4"/>
     </row>
-    <row r="823" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="823" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C823" s="4"/>
     </row>
-    <row r="824" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="824" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C824" s="4"/>
     </row>
-    <row r="825" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="825" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C825" s="4"/>
     </row>
-    <row r="826" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="826" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C826" s="4"/>
     </row>
-    <row r="827" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="827" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C827" s="4"/>
     </row>
-    <row r="828" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="828" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C828" s="4"/>
     </row>
-    <row r="829" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="829" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C829" s="4"/>
     </row>
-    <row r="830" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="830" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C830" s="4"/>
     </row>
-    <row r="831" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="831" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C831" s="4"/>
     </row>
-    <row r="832" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="832" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C832" s="4"/>
     </row>
-    <row r="833" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="833" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C833" s="4"/>
     </row>
-    <row r="834" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="834" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C834" s="4"/>
     </row>
-    <row r="835" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="835" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C835" s="4"/>
     </row>
-    <row r="836" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="836" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C836" s="4"/>
     </row>
-    <row r="837" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="837" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C837" s="4"/>
     </row>
-    <row r="838" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="838" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C838" s="4"/>
     </row>
-    <row r="839" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="839" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C839" s="4"/>
     </row>
-    <row r="840" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="840" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C840" s="4"/>
     </row>
-    <row r="841" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="841" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C841" s="4"/>
     </row>
-    <row r="842" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="842" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C842" s="4"/>
     </row>
-    <row r="843" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="843" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C843" s="4"/>
     </row>
-    <row r="844" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="844" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C844" s="4"/>
     </row>
-    <row r="845" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="845" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C845" s="4"/>
     </row>
-    <row r="846" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="846" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C846" s="4"/>
     </row>
-    <row r="847" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="847" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C847" s="4"/>
     </row>
-    <row r="848" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="848" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C848" s="4"/>
     </row>
-    <row r="849" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="849" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C849" s="4"/>
     </row>
-    <row r="850" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="850" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C850" s="4"/>
     </row>
-    <row r="851" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="851" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C851" s="4"/>
     </row>
-    <row r="852" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="852" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C852" s="4"/>
     </row>
-    <row r="853" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="853" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C853" s="4"/>
     </row>
-    <row r="854" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="854" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C854" s="4"/>
     </row>
-    <row r="855" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="855" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C855" s="4"/>
     </row>
-    <row r="856" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="856" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C856" s="4"/>
     </row>
-    <row r="857" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="857" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C857" s="4"/>
     </row>
-    <row r="858" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="858" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C858" s="4"/>
     </row>
-    <row r="859" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="859" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C859" s="4"/>
     </row>
-    <row r="860" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="860" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C860" s="4"/>
     </row>
-    <row r="861" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="861" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C861" s="4"/>
     </row>
-    <row r="862" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="862" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C862" s="4"/>
     </row>
-    <row r="863" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="863" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C863" s="4"/>
     </row>
-    <row r="864" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="864" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C864" s="4"/>
     </row>
-    <row r="865" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="865" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C865" s="4"/>
     </row>
-    <row r="866" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="866" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C866" s="4"/>
     </row>
-    <row r="867" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="867" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C867" s="4"/>
     </row>
-    <row r="868" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="868" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C868" s="4"/>
     </row>
-    <row r="869" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="869" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C869" s="4"/>
     </row>
-    <row r="870" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="870" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C870" s="4"/>
     </row>
-    <row r="871" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="871" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C871" s="4"/>
     </row>
-    <row r="872" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="872" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C872" s="4"/>
     </row>
-    <row r="873" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="873" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C873" s="4"/>
     </row>
-    <row r="874" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="874" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C874" s="4"/>
     </row>
-    <row r="875" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="875" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C875" s="4"/>
     </row>
-    <row r="876" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="876" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C876" s="4"/>
     </row>
-    <row r="877" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="877" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C877" s="4"/>
     </row>
-    <row r="878" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="878" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C878" s="4"/>
     </row>
-    <row r="879" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="879" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C879" s="4"/>
     </row>
-    <row r="880" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="880" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C880" s="4"/>
     </row>
-    <row r="881" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="881" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C881" s="4"/>
     </row>
-    <row r="882" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="882" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C882" s="4"/>
     </row>
-    <row r="883" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="883" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C883" s="4"/>
     </row>
-    <row r="884" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="884" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C884" s="4"/>
     </row>
-    <row r="885" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="885" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C885" s="4"/>
     </row>
-    <row r="886" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="886" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C886" s="4"/>
     </row>
-    <row r="887" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="887" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C887" s="4"/>
     </row>
-    <row r="888" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="888" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C888" s="4"/>
     </row>
-    <row r="889" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="889" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C889" s="4"/>
     </row>
-    <row r="890" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="890" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C890" s="4"/>
     </row>
-    <row r="891" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="891" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C891" s="4"/>
     </row>
-    <row r="892" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="892" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C892" s="4"/>
     </row>
-    <row r="893" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="893" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C893" s="4"/>
     </row>
-    <row r="894" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="894" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C894" s="4"/>
     </row>
-    <row r="895" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="895" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C895" s="4"/>
     </row>
-    <row r="896" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="896" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C896" s="4"/>
     </row>
-    <row r="897" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="897" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C897" s="4"/>
     </row>
-    <row r="898" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="898" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C898" s="4"/>
     </row>
-    <row r="899" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="899" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C899" s="4"/>
     </row>
-    <row r="900" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="900" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C900" s="4"/>
     </row>
-    <row r="901" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="901" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C901" s="4"/>
     </row>
-    <row r="902" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="902" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C902" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EtherCAT sample_app.xlsx file is now readable. Updated Git attribute for xlsx extention. [MH3-43715]
</commit_message>
<xml_diff>
--- a/apps/ethercat_counter_foe_app/firmware/src/slave_stack/sample_app.xlsx
+++ b/apps/ethercat_counter_foe_app/firmware/src/slave_stack/sample_app.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\microchip\h3\new_ethercat\ethercat\apps\ethercat_counter_foe_app\firmware\src\slave_stack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\microchip\h3\ethercat\apps\ethercat_counter_foe_app\firmware\src\slave_stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3298A-B458-4463-AD2D-547D1A138D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C3C00-00F4-4875-A861-9910802989A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -800,7 +800,7 @@
   <dimension ref="A1:T902"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1:P6"/>
     </sheetView>
   </sheetViews>

</xml_diff>